<commit_message>
Aggiornato report-checklist colonna K
S1#111EUROMEDICAL
EUROMEDICAL
MEDIWEB
1.0
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111EUROMEDICAL/EUROMEDICAL/MEDIWEB/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111EUROMEDICAL/EUROMEDICAL/MEDIWEB/1.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="829" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="294">
   <si>
     <t>ID</t>
   </si>
@@ -675,9 +675,6 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>Le sezioni opzionali richieste vengono utilizzate solo in parte (utilizzando  /ClinicalDocument/component/structuredBody/component/section/text), in quanto alcune informazioni vengono sintetizzate in fase di redazione della LDO e quindi gestite in modo non strutturato.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LDO_CT4</t>
   </si>
   <si>
@@ -721,9 +718,6 @@
 Il Documento CDA2 Verbale di Pronto Soccorso dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>Alcune delle sezioni opzionali richieste vengono incluse nel verbale solo nella loro componente narrativa (/ClinicalDocument/component/structuredBody/component/section/component/section/text) in quanto l'informazione viene sintetizzata in fase di redazione del verbale di pronto soccorso.</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_VPS_CT3</t>
   </si>
   <si>
@@ -748,9 +742,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 13" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento. </t>
   </si>
   <si>
-    <t>Campi opzionali non gestiti</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LDO_CT14_KO</t>
   </si>
   <si>
@@ -852,9 +843,6 @@
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 17" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>Campo opzionale non gestito</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_VPS_CT18_KO</t>
   </si>
   <si>
@@ -874,9 +862,6 @@
   <si>
     <t>Viene richiamato il servizio di validazione "https://&lt;HOST&gt;:&lt;PORT&gt;/v&lt;major&gt;/documents/validation" al fine di testare la gestione degli errori semantici sui Dati (status code 422), secondo quanto descritto in https://github.com/ministero-salute/it-fse-support/tree/main/doc/integrazione-gateway. 
 I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso nella sezione "CASO DI TEST 21" riportata nei documenti "casi di test VPS" e "CDA2_Verbale_Pronto_Soccorso_KO" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
-  </si>
-  <si>
-    <t>Sezione opzionale non gestita</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_VPS_CT24_KO</t>
@@ -1008,9 +993,6 @@
   </si>
   <si>
     <t>VALIDAZIONE_VPS_TIMEOUT</t>
-  </si>
-  <si>
-    <t>Le sezioni opzionali richieste vengono popolate nella loro componente narrativa (utilizzando /ClinicalDocument/component/structuredBody/component/section/text) ma non nella loro forma strutturata, in quanto alcune delle informazioni afferenti vengono sintetizzate in fase di redazione della LDO e quindi gestite in modo non strutturato.</t>
   </si>
   <si>
     <r>
@@ -1061,9 +1043,6 @@
 E' facoltà della singola azienda, secondo le proprie policy, rendere ciascuna tipologia di errore (come timeout, jwt, sintassi, vocabolario, semantica) visibile o meno all'operatore e, nel caso, se renderla bloccante o meno.</t>
   </si>
   <si>
-    <t>Campi opzionale non gestito</t>
-  </si>
-  <si>
     <t>Euromedical Service S.r.l.</t>
   </si>
   <si>
@@ -1242,6 +1221,9 @@
   </si>
   <si>
     <t>f1b6258b62dda099</t>
+  </si>
+  <si>
+    <t>Tipo Documento non gestito</t>
   </si>
 </sst>
 </file>
@@ -1914,14 +1896,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:T111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="E8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="H22" sqref="H22"/>
+      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1950,7 +1931,7 @@
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="31" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D2" s="32"/>
     </row>
@@ -1960,7 +1941,7 @@
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="35" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D3" s="30"/>
     </row>
@@ -1968,7 +1949,7 @@
       <c r="A4" s="38"/>
       <c r="B4" s="39"/>
       <c r="C4" s="35" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="D4" s="30"/>
     </row>
@@ -1976,7 +1957,7 @@
       <c r="A5" s="40"/>
       <c r="B5" s="41"/>
       <c r="C5" s="35" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="D5" s="30"/>
     </row>
@@ -2047,7 +2028,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -2070,7 +2051,9 @@
       <c r="J8" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K8" s="9"/>
+      <c r="K8" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -2083,7 +2066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -2107,7 +2090,7 @@
         <v>146</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>236</v>
+        <v>293</v>
       </c>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
@@ -2121,7 +2104,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -2145,7 +2128,7 @@
         <v>146</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>149</v>
+        <v>293</v>
       </c>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
@@ -2159,7 +2142,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -2170,10 +2153,10 @@
         <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>151</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
@@ -2183,7 +2166,7 @@
         <v>146</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>149</v>
+        <v>293</v>
       </c>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
@@ -2197,7 +2180,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -2220,7 +2203,9 @@
       <c r="J12" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K12" s="9"/>
+      <c r="K12" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -2233,7 +2218,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -2244,10 +2229,10 @@
         <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>152</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>153</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
@@ -2256,8 +2241,8 @@
       <c r="J13" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K13" s="6" t="s">
-        <v>154</v>
+      <c r="K13" s="9" t="s">
+        <v>293</v>
       </c>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
@@ -2271,7 +2256,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -2282,10 +2267,10 @@
         <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
@@ -2294,8 +2279,8 @@
       <c r="J14" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K14" s="6" t="s">
-        <v>154</v>
+      <c r="K14" s="9" t="s">
+        <v>293</v>
       </c>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -2309,7 +2294,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -2320,10 +2305,10 @@
         <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
@@ -2332,8 +2317,8 @@
       <c r="J15" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K15" s="6" t="s">
-        <v>154</v>
+      <c r="K15" s="9" t="s">
+        <v>293</v>
       </c>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
@@ -2347,7 +2332,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="4">
         <v>24</v>
       </c>
@@ -2370,7 +2355,9 @@
       <c r="J16" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K16" s="9"/>
+      <c r="K16" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -2383,7 +2370,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="4">
         <v>25</v>
       </c>
@@ -2394,10 +2381,10 @@
         <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
@@ -2407,7 +2394,7 @@
         <v>146</v>
       </c>
       <c r="K17" s="9" t="s">
-        <v>161</v>
+        <v>293</v>
       </c>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
@@ -2421,7 +2408,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="4">
         <v>26</v>
       </c>
@@ -2432,10 +2419,10 @@
         <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
@@ -2445,7 +2432,7 @@
         <v>146</v>
       </c>
       <c r="K18" s="9" t="s">
-        <v>161</v>
+        <v>293</v>
       </c>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
@@ -2459,7 +2446,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="4">
         <v>27</v>
       </c>
@@ -2470,10 +2457,10 @@
         <v>29</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
@@ -2483,7 +2470,7 @@
         <v>146</v>
       </c>
       <c r="K19" s="9" t="s">
-        <v>161</v>
+        <v>293</v>
       </c>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
@@ -2497,7 +2484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="4">
         <v>29</v>
       </c>
@@ -2520,7 +2507,9 @@
       <c r="J20" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K20" s="9"/>
+      <c r="K20" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
@@ -2533,7 +2522,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="210.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:20" ht="210.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="4">
         <v>31</v>
       </c>
@@ -2556,13 +2545,15 @@
       <c r="J21" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K21" s="9"/>
+      <c r="K21" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q21" s="9"/>
       <c r="R21" s="10"/>
@@ -2591,10 +2582,10 @@
         <v>45092</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="I22" s="21" t="s">
         <v>34</v>
@@ -2610,13 +2601,13 @@
         <v>24</v>
       </c>
       <c r="N22" s="22" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O22" s="22" t="s">
         <v>24</v>
       </c>
       <c r="P22" s="22" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q22" s="22"/>
       <c r="R22" s="23"/>
@@ -2625,7 +2616,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="203.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:20" ht="203.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="4">
         <v>35</v>
       </c>
@@ -2648,7 +2639,9 @@
       <c r="J23" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K23" s="9"/>
+      <c r="K23" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -2661,7 +2654,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="4">
         <v>37</v>
       </c>
@@ -2684,7 +2677,9 @@
       <c r="J24" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K24" s="9"/>
+      <c r="K24" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
@@ -2697,7 +2692,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="4">
         <v>39</v>
       </c>
@@ -2720,7 +2715,9 @@
       <c r="J25" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K25" s="9"/>
+      <c r="K25" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -2753,10 +2750,10 @@
         <v>45092</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>34</v>
@@ -2772,13 +2769,13 @@
         <v>24</v>
       </c>
       <c r="N26" s="22" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O26" s="22" t="s">
         <v>24</v>
       </c>
       <c r="P26" s="22" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q26" s="22"/>
       <c r="R26" s="23"/>
@@ -2787,7 +2784,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="189" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:20" ht="189" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="4">
         <v>43</v>
       </c>
@@ -2810,7 +2807,9 @@
       <c r="J27" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K27" s="9"/>
+      <c r="K27" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
@@ -2823,7 +2822,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="4">
         <v>45</v>
       </c>
@@ -2834,10 +2833,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
@@ -2846,13 +2845,15 @@
       <c r="J28" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K28" s="9"/>
+      <c r="K28" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q28" s="9"/>
       <c r="R28" s="10" t="s">
@@ -2863,7 +2864,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="142.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:20" ht="142.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="4">
         <v>47</v>
       </c>
@@ -2874,10 +2875,10 @@
         <v>26</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
@@ -2886,13 +2887,15 @@
       <c r="J29" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K29" s="9"/>
+      <c r="K29" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q29" s="9"/>
       <c r="R29" s="10" t="s">
@@ -2903,7 +2906,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="136.5" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:20" ht="136.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="4">
         <v>48</v>
       </c>
@@ -2914,10 +2917,10 @@
         <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
@@ -2926,13 +2929,15 @@
       <c r="J30" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K30" s="9"/>
+      <c r="K30" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q30" s="9"/>
       <c r="R30" s="10" t="s">
@@ -2943,7 +2948,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="4">
         <v>51</v>
       </c>
@@ -2954,10 +2959,10 @@
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
@@ -2966,13 +2971,15 @@
       <c r="J31" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K31" s="9"/>
+      <c r="K31" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q31" s="9"/>
       <c r="R31" s="10" t="s">
@@ -2983,7 +2990,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="225.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:20" ht="225.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="4">
         <v>63</v>
       </c>
@@ -3006,7 +3013,9 @@
       <c r="J32" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K32" s="9"/>
+      <c r="K32" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
@@ -3019,7 +3028,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="4">
         <v>64</v>
       </c>
@@ -3042,7 +3051,9 @@
       <c r="J33" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K33" s="9"/>
+      <c r="K33" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -3055,7 +3066,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="4">
         <v>65</v>
       </c>
@@ -3078,7 +3089,9 @@
       <c r="J34" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K34" s="9"/>
+      <c r="K34" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
@@ -3091,7 +3104,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="4">
         <v>66</v>
       </c>
@@ -3114,7 +3127,9 @@
       <c r="J35" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K35" s="9"/>
+      <c r="K35" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
@@ -3127,7 +3142,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="4">
         <v>67</v>
       </c>
@@ -3150,7 +3165,9 @@
       <c r="J36" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K36" s="9"/>
+      <c r="K36" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
@@ -3163,7 +3180,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="4">
         <v>68</v>
       </c>
@@ -3186,7 +3203,9 @@
       <c r="J37" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K37" s="9"/>
+      <c r="K37" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
@@ -3199,7 +3218,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="4">
         <v>69</v>
       </c>
@@ -3222,7 +3241,9 @@
       <c r="J38" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K38" s="9"/>
+      <c r="K38" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
@@ -3235,7 +3256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="4">
         <v>70</v>
       </c>
@@ -3258,7 +3279,9 @@
       <c r="J39" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K39" s="9"/>
+      <c r="K39" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
@@ -3271,7 +3294,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="4">
         <v>71</v>
       </c>
@@ -3282,10 +3305,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
@@ -3295,7 +3318,7 @@
         <v>146</v>
       </c>
       <c r="K40" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
@@ -3309,7 +3332,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="4">
         <v>72</v>
       </c>
@@ -3320,10 +3343,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
@@ -3333,7 +3356,7 @@
         <v>146</v>
       </c>
       <c r="K41" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
@@ -3347,7 +3370,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="4">
         <v>73</v>
       </c>
@@ -3358,10 +3381,10 @@
         <v>21</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
@@ -3371,7 +3394,7 @@
         <v>146</v>
       </c>
       <c r="K42" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
@@ -3385,7 +3408,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="4">
         <v>74</v>
       </c>
@@ -3396,10 +3419,10 @@
         <v>21</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
@@ -3409,7 +3432,7 @@
         <v>146</v>
       </c>
       <c r="K43" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
@@ -3423,7 +3446,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="4">
         <v>75</v>
       </c>
@@ -3446,7 +3469,9 @@
       <c r="J44" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K44" s="9"/>
+      <c r="K44" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
@@ -3459,7 +3484,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="4">
         <v>76</v>
       </c>
@@ -3482,7 +3507,9 @@
       <c r="J45" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K45" s="9"/>
+      <c r="K45" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
@@ -3495,7 +3522,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="4">
         <v>77</v>
       </c>
@@ -3518,7 +3545,9 @@
       <c r="J46" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K46" s="9"/>
+      <c r="K46" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
@@ -3531,7 +3560,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="4">
         <v>78</v>
       </c>
@@ -3554,7 +3583,9 @@
       <c r="J47" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K47" s="9"/>
+      <c r="K47" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
@@ -3567,7 +3598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="4">
         <v>79</v>
       </c>
@@ -3590,7 +3621,9 @@
       <c r="J48" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K48" s="9"/>
+      <c r="K48" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
@@ -3603,7 +3636,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="4">
         <v>80</v>
       </c>
@@ -3626,7 +3659,9 @@
       <c r="J49" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K49" s="9"/>
+      <c r="K49" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
@@ -3639,7 +3674,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="4">
         <v>81</v>
       </c>
@@ -3662,7 +3697,9 @@
       <c r="J50" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K50" s="9"/>
+      <c r="K50" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
       <c r="N50" s="9"/>
@@ -3675,7 +3712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="4">
         <v>82</v>
       </c>
@@ -3686,10 +3723,10 @@
         <v>26</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
@@ -3699,7 +3736,7 @@
         <v>146</v>
       </c>
       <c r="K51" s="9" t="s">
-        <v>195</v>
+        <v>293</v>
       </c>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
@@ -3713,7 +3750,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="4">
         <v>83</v>
       </c>
@@ -3736,7 +3773,9 @@
       <c r="J52" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K52" s="9"/>
+      <c r="K52" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
@@ -3749,7 +3788,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="4">
         <v>84</v>
       </c>
@@ -3772,7 +3811,9 @@
       <c r="J53" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K53" s="9"/>
+      <c r="K53" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
@@ -3785,7 +3826,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="4">
         <v>85</v>
       </c>
@@ -3808,7 +3849,9 @@
       <c r="J54" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K54" s="9"/>
+      <c r="K54" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
@@ -3821,7 +3864,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="4">
         <v>86</v>
       </c>
@@ -3832,10 +3875,10 @@
         <v>26</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
@@ -3845,7 +3888,7 @@
         <v>146</v>
       </c>
       <c r="K55" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
@@ -3859,7 +3902,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="4">
         <v>87</v>
       </c>
@@ -3870,10 +3913,10 @@
         <v>26</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
@@ -3883,7 +3926,7 @@
         <v>146</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
@@ -3897,7 +3940,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="4">
         <v>88</v>
       </c>
@@ -3908,10 +3951,10 @@
         <v>26</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
@@ -3921,7 +3964,7 @@
         <v>146</v>
       </c>
       <c r="K57" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
@@ -3935,7 +3978,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="4">
         <v>89</v>
       </c>
@@ -3946,10 +3989,10 @@
         <v>26</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
@@ -3959,7 +4002,7 @@
         <v>146</v>
       </c>
       <c r="K58" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
@@ -3973,7 +4016,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="4">
         <v>90</v>
       </c>
@@ -3984,10 +4027,10 @@
         <v>26</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
@@ -3997,7 +4040,7 @@
         <v>146</v>
       </c>
       <c r="K59" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
@@ -4011,7 +4054,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="4">
         <v>91</v>
       </c>
@@ -4022,10 +4065,10 @@
         <v>26</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
@@ -4035,7 +4078,7 @@
         <v>146</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
@@ -4049,7 +4092,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="4">
         <v>92</v>
       </c>
@@ -4060,10 +4103,10 @@
         <v>26</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
@@ -4073,7 +4116,7 @@
         <v>146</v>
       </c>
       <c r="K61" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
@@ -4087,7 +4130,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="4">
         <v>93</v>
       </c>
@@ -4098,10 +4141,10 @@
         <v>26</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
@@ -4111,7 +4154,7 @@
         <v>146</v>
       </c>
       <c r="K62" s="9" t="s">
-        <v>195</v>
+        <v>293</v>
       </c>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
@@ -4125,7 +4168,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="63" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="4">
         <v>122</v>
       </c>
@@ -4148,7 +4191,9 @@
       <c r="J63" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K63" s="9"/>
+      <c r="K63" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
@@ -4161,7 +4206,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="4">
         <v>123</v>
       </c>
@@ -4184,7 +4229,9 @@
       <c r="J64" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K64" s="9"/>
+      <c r="K64" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
@@ -4197,7 +4244,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="4">
         <v>124</v>
       </c>
@@ -4220,7 +4267,9 @@
       <c r="J65" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K65" s="9"/>
+      <c r="K65" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
@@ -4233,7 +4282,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="4">
         <v>125</v>
       </c>
@@ -4256,7 +4305,9 @@
       <c r="J66" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K66" s="9"/>
+      <c r="K66" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
@@ -4269,7 +4320,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="4">
         <v>126</v>
       </c>
@@ -4292,7 +4343,9 @@
       <c r="J67" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K67" s="9"/>
+      <c r="K67" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
@@ -4305,7 +4358,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="4">
         <v>127</v>
       </c>
@@ -4328,7 +4381,9 @@
       <c r="J68" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K68" s="9"/>
+      <c r="K68" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
@@ -4341,7 +4396,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="4">
         <v>128</v>
       </c>
@@ -4364,7 +4419,9 @@
       <c r="J69" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K69" s="9"/>
+      <c r="K69" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
       <c r="N69" s="9"/>
@@ -4377,7 +4434,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="4">
         <v>129</v>
       </c>
@@ -4400,7 +4457,9 @@
       <c r="J70" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K70" s="9"/>
+      <c r="K70" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
       <c r="N70" s="9"/>
@@ -4413,7 +4472,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="4">
         <v>130</v>
       </c>
@@ -4436,7 +4495,9 @@
       <c r="J71" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K71" s="9"/>
+      <c r="K71" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
@@ -4449,7 +4510,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="4">
         <v>131</v>
       </c>
@@ -4472,7 +4533,9 @@
       <c r="J72" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K72" s="9"/>
+      <c r="K72" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
       <c r="N72" s="9"/>
@@ -4485,7 +4548,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="4">
         <v>132</v>
       </c>
@@ -4508,7 +4571,9 @@
       <c r="J73" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K73" s="9"/>
+      <c r="K73" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
       <c r="N73" s="9"/>
@@ -4521,7 +4586,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="4">
         <v>133</v>
       </c>
@@ -4544,7 +4609,9 @@
       <c r="J74" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K74" s="9"/>
+      <c r="K74" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>
@@ -4557,7 +4624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="4">
         <v>134</v>
       </c>
@@ -4568,10 +4635,10 @@
         <v>29</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
@@ -4581,7 +4648,7 @@
         <v>146</v>
       </c>
       <c r="K75" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
@@ -4595,7 +4662,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="4">
         <v>135</v>
       </c>
@@ -4606,10 +4673,10 @@
         <v>29</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
@@ -4619,7 +4686,7 @@
         <v>146</v>
       </c>
       <c r="K76" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
@@ -4633,7 +4700,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="4">
         <v>136</v>
       </c>
@@ -4644,10 +4711,10 @@
         <v>29</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
@@ -4657,7 +4724,7 @@
         <v>146</v>
       </c>
       <c r="K77" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
@@ -4671,7 +4738,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="4">
         <v>137</v>
       </c>
@@ -4694,7 +4761,9 @@
       <c r="J78" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K78" s="9"/>
+      <c r="K78" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
       <c r="N78" s="9"/>
@@ -4707,7 +4776,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="4">
         <v>138</v>
       </c>
@@ -4718,10 +4787,10 @@
         <v>29</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
@@ -4731,7 +4800,7 @@
         <v>146</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
@@ -4745,7 +4814,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="4">
         <v>139</v>
       </c>
@@ -4768,7 +4837,9 @@
       <c r="J80" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K80" s="9"/>
+      <c r="K80" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L80" s="9"/>
       <c r="M80" s="9"/>
       <c r="N80" s="9"/>
@@ -4781,7 +4852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="4">
         <v>140</v>
       </c>
@@ -4804,7 +4875,9 @@
       <c r="J81" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K81" s="9"/>
+      <c r="K81" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
       <c r="N81" s="9"/>
@@ -4817,7 +4890,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="4">
         <v>141</v>
       </c>
@@ -4828,10 +4901,10 @@
         <v>29</v>
       </c>
       <c r="D82" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
@@ -4841,7 +4914,7 @@
         <v>146</v>
       </c>
       <c r="K82" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
@@ -4855,7 +4928,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="4">
         <v>142</v>
       </c>
@@ -4878,7 +4951,9 @@
       <c r="J83" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K83" s="9"/>
+      <c r="K83" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
@@ -4891,7 +4966,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="4">
         <v>143</v>
       </c>
@@ -4914,7 +4989,9 @@
       <c r="J84" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K84" s="9"/>
+      <c r="K84" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
       <c r="N84" s="9"/>
@@ -4927,7 +5004,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="145.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:20" ht="145.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A85" s="4">
         <v>144</v>
       </c>
@@ -4950,7 +5027,9 @@
       <c r="J85" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K85" s="9"/>
+      <c r="K85" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
@@ -4963,7 +5042,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="4">
         <v>145</v>
       </c>
@@ -4974,10 +5053,10 @@
         <v>29</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
@@ -4987,7 +5066,7 @@
         <v>146</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>168</v>
+        <v>293</v>
       </c>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
@@ -5001,7 +5080,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="87" spans="1:20" ht="160" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:20" ht="160" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="4">
         <v>146</v>
       </c>
@@ -5012,10 +5091,10 @@
         <v>29</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E87" s="6" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
@@ -5025,7 +5104,7 @@
         <v>146</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>239</v>
+        <v>293</v>
       </c>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
@@ -5059,13 +5138,13 @@
         <v>45055</v>
       </c>
       <c r="G88" s="21" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="H88" s="21" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I88" s="21" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="J88" s="22" t="s">
         <v>24</v>
@@ -5094,22 +5173,22 @@
         <v>37</v>
       </c>
       <c r="D89" s="18" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F89" s="20">
         <v>45058</v>
       </c>
       <c r="G89" s="21" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="H89" s="21" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="I89" s="21" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="J89" s="27" t="s">
         <v>24</v>
@@ -5138,28 +5217,28 @@
         <v>37</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="F90" s="7">
         <v>45058</v>
       </c>
       <c r="G90" s="8" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H90" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="I90" s="8" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="J90" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
@@ -5184,28 +5263,28 @@
         <v>37</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="F91" s="7">
         <v>45058</v>
       </c>
       <c r="G91" s="8" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="H91" s="8" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="I91" s="8" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="J91" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
@@ -5239,13 +5318,13 @@
         <v>45058</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="J92" s="9" t="s">
         <v>24</v>
@@ -5258,13 +5337,13 @@
         <v>24</v>
       </c>
       <c r="N92" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O92" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P92" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q92" s="9"/>
       <c r="R92" s="10"/>
@@ -5293,13 +5372,13 @@
         <v>45058</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="J93" s="9" t="s">
         <v>24</v>
@@ -5312,13 +5391,13 @@
         <v>24</v>
       </c>
       <c r="N93" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O93" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P93" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q93" s="9"/>
       <c r="R93" s="10"/>
@@ -5347,13 +5426,13 @@
         <v>45058</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="H94" s="8" t="s">
         <v>125</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="J94" s="9" t="s">
         <v>24</v>
@@ -5366,13 +5445,13 @@
         <v>24</v>
       </c>
       <c r="N94" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O94" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P94" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q94" s="9"/>
       <c r="R94" s="10"/>
@@ -5401,13 +5480,13 @@
         <v>45058</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="J95" s="9" t="s">
         <v>24</v>
@@ -5420,13 +5499,13 @@
         <v>24</v>
       </c>
       <c r="N95" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O95" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P95" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q95" s="9"/>
       <c r="R95" s="10"/>
@@ -5455,13 +5534,13 @@
         <v>45058</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J96" s="9" t="s">
         <v>24</v>
@@ -5474,13 +5553,13 @@
         <v>24</v>
       </c>
       <c r="N96" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O96" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P96" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q96" s="9"/>
       <c r="R96" s="10"/>
@@ -5509,13 +5588,13 @@
         <v>45058</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="J97" s="9" t="s">
         <v>24</v>
@@ -5528,13 +5607,13 @@
         <v>24</v>
       </c>
       <c r="N97" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O97" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P97" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q97" s="9"/>
       <c r="R97" s="10"/>
@@ -5554,41 +5633,41 @@
         <v>37</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E98" s="6" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="F98" s="7">
         <v>45058</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="J98" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K98" s="9"/>
       <c r="L98" s="9" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="M98" s="9" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="N98" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O98" s="9" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="P98" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q98" s="9"/>
       <c r="R98" s="10"/>
@@ -5608,41 +5687,41 @@
         <v>37</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="F99" s="7">
         <v>45058</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="J99" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K99" s="9"/>
       <c r="L99" s="9" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="M99" s="9" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="N99" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O99" s="9" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="P99" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q99" s="9"/>
       <c r="R99" s="10"/>
@@ -5671,13 +5750,13 @@
         <v>45058</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="J100" s="9" t="s">
         <v>24</v>
@@ -5690,13 +5769,13 @@
         <v>24</v>
       </c>
       <c r="N100" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O100" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P100" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q100" s="9"/>
       <c r="R100" s="10"/>
@@ -5725,13 +5804,13 @@
         <v>45058</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="I101" s="8" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="J101" s="9" t="s">
         <v>24</v>
@@ -5744,13 +5823,13 @@
         <v>24</v>
       </c>
       <c r="N101" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O101" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P101" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q101" s="9"/>
       <c r="R101" s="10"/>
@@ -5779,13 +5858,13 @@
         <v>45058</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="J102" s="9" t="s">
         <v>24</v>
@@ -5798,13 +5877,13 @@
         <v>24</v>
       </c>
       <c r="N102" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O102" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P102" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q102" s="9"/>
       <c r="R102" s="10"/>
@@ -5824,22 +5903,22 @@
         <v>37</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="E103" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="F103" s="7">
         <v>45058</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="J103" s="9" t="s">
         <v>24</v>
@@ -5852,13 +5931,13 @@
         <v>24</v>
       </c>
       <c r="N103" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O103" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P103" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q103" s="9"/>
       <c r="R103" s="10"/>
@@ -5887,13 +5966,13 @@
         <v>45058</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="J104" s="9" t="s">
         <v>24</v>
@@ -5906,13 +5985,13 @@
         <v>24</v>
       </c>
       <c r="N104" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O104" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P104" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q104" s="9"/>
       <c r="R104" s="10"/>
@@ -5921,7 +6000,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="105" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A105" s="4">
         <v>164</v>
       </c>
@@ -5932,10 +6011,10 @@
         <v>37</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="E105" s="6" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
@@ -5945,7 +6024,7 @@
         <v>146</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
@@ -5959,7 +6038,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="106" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="4">
         <v>165</v>
       </c>
@@ -5970,10 +6049,10 @@
         <v>37</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="E106" s="6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
@@ -5983,7 +6062,7 @@
         <v>146</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L106" s="9"/>
       <c r="M106" s="9"/>
@@ -5997,7 +6076,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="107" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A107" s="4">
         <v>166</v>
       </c>
@@ -6008,10 +6087,10 @@
         <v>37</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="E107" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
@@ -6021,7 +6100,7 @@
         <v>146</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L107" s="9"/>
       <c r="M107" s="9"/>
@@ -6035,7 +6114,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="108" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="4">
         <v>167</v>
       </c>
@@ -6046,10 +6125,10 @@
         <v>37</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E108" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
@@ -6059,7 +6138,7 @@
         <v>146</v>
       </c>
       <c r="K108" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L108" s="9"/>
       <c r="M108" s="9"/>
@@ -6073,7 +6152,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="109" spans="1:20" ht="174.5" hidden="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:20" ht="174.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A109" s="4">
         <v>168</v>
       </c>
@@ -6084,10 +6163,10 @@
         <v>37</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="E109" s="6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
@@ -6097,7 +6176,7 @@
         <v>146</v>
       </c>
       <c r="K109" s="9" t="s">
-        <v>202</v>
+        <v>293</v>
       </c>
       <c r="L109" s="9"/>
       <c r="M109" s="9"/>
@@ -6131,13 +6210,13 @@
         <v>45058</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="J110" s="9" t="s">
         <v>24</v>
@@ -6150,13 +6229,13 @@
         <v>24</v>
       </c>
       <c r="N110" s="9" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="O110" s="9" t="s">
         <v>24</v>
       </c>
       <c r="P110" s="9" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="Q110" s="9"/>
       <c r="R110" s="10"/>
@@ -6169,13 +6248,6 @@
       <c r="J111" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A7:T110">
-    <filterColumn colId="9">
-      <filters>
-        <filter val="SI"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <mergeCells count="7">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="C2:D2"/>

</xml_diff>

<commit_message>
Eliminate colonne come da indicazioni
S1#111EUROMEDICAL
EUROMEDICAL
MEDIWEB
1.0
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111EUROMEDICAL/EUROMEDICAL/MEDIWEB/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111EUROMEDICAL/EUROMEDICAL/MEDIWEB/1.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="878" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="293">
   <si>
     <t>ID</t>
   </si>
@@ -664,9 +664,6 @@
 Il Documento CDA2 Lettera Dimissione Ospedaliera dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test LDO" e "CDA2_Lettera di Dimissione Ospedaliera_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_LDO_CT3</t>
   </si>
   <si>
@@ -1223,7 +1220,7 @@
     <t>f1b6258b62dda099</t>
   </si>
   <si>
-    <t>Tipo Documento non gestito</t>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1899,10 +1896,10 @@
   <dimension ref="A1:T111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="67" zoomScaleNormal="67" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="G26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="A26" sqref="A26"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1931,7 +1928,7 @@
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="31" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D2" s="32"/>
     </row>
@@ -1941,7 +1938,7 @@
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="35" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D3" s="30"/>
     </row>
@@ -1949,7 +1946,7 @@
       <c r="A4" s="38"/>
       <c r="B4" s="39"/>
       <c r="C4" s="35" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D4" s="30"/>
     </row>
@@ -1957,7 +1954,7 @@
       <c r="A5" s="40"/>
       <c r="B5" s="41"/>
       <c r="C5" s="35" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D5" s="30"/>
     </row>
@@ -2049,11 +2046,9 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>293</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="K8" s="9"/>
       <c r="L8" s="9"/>
       <c r="M8" s="9"/>
       <c r="N8" s="9"/>
@@ -2086,12 +2081,8 @@
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
-      <c r="J9" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K9" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="9"/>
       <c r="M9" s="9"/>
       <c r="N9" s="9"/>
@@ -2115,21 +2106,17 @@
         <v>21</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>147</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>148</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
       <c r="I10" s="8"/>
-      <c r="J10" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="9"/>
       <c r="N10" s="9"/>
@@ -2153,21 +2140,17 @@
         <v>21</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
-      <c r="J11" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K11" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="9"/>
       <c r="N11" s="9"/>
@@ -2200,12 +2183,8 @@
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
-      <c r="J12" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K12" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="9"/>
       <c r="N12" s="9"/>
@@ -2229,21 +2208,17 @@
         <v>26</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E13" s="6" t="s">
         <v>151</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
-      <c r="J13" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K13" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
       <c r="L13" s="9"/>
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
@@ -2267,21 +2242,17 @@
         <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>155</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
       <c r="I14" s="8"/>
-      <c r="J14" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
@@ -2305,21 +2276,17 @@
         <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>156</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>157</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
       <c r="I15" s="8"/>
-      <c r="J15" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K15" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="9"/>
       <c r="N15" s="9"/>
@@ -2352,12 +2319,8 @@
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
       <c r="I16" s="8"/>
-      <c r="J16" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K16" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J16" s="9"/>
+      <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="9"/>
       <c r="N16" s="9"/>
@@ -2381,21 +2344,17 @@
         <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>158</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>159</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
       <c r="I17" s="8"/>
-      <c r="J17" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
       <c r="L17" s="9"/>
       <c r="M17" s="9"/>
       <c r="N17" s="9"/>
@@ -2419,21 +2378,17 @@
         <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>160</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
-      <c r="J18" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K18" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="9"/>
       <c r="N18" s="9"/>
@@ -2457,21 +2412,17 @@
         <v>29</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>162</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>163</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
-      <c r="J19" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K19" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="9"/>
       <c r="N19" s="9"/>
@@ -2504,12 +2455,8 @@
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-      <c r="J20" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K20" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="9"/>
       <c r="M20" s="9"/>
       <c r="N20" s="9"/>
@@ -2542,18 +2489,14 @@
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-      <c r="J21" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K21" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="9"/>
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q21" s="9"/>
       <c r="R21" s="10"/>
@@ -2582,10 +2525,10 @@
         <v>45092</v>
       </c>
       <c r="G22" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="H22" s="21" t="s">
         <v>289</v>
-      </c>
-      <c r="H22" s="21" t="s">
-        <v>290</v>
       </c>
       <c r="I22" s="21" t="s">
         <v>34</v>
@@ -2601,13 +2544,13 @@
         <v>24</v>
       </c>
       <c r="N22" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="O22" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="P22" s="22" t="s">
         <v>231</v>
-      </c>
-      <c r="O22" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P22" s="22" t="s">
-        <v>232</v>
       </c>
       <c r="Q22" s="22"/>
       <c r="R22" s="23"/>
@@ -2636,12 +2579,8 @@
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
-      <c r="J23" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K23" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="9"/>
       <c r="N23" s="9"/>
@@ -2674,12 +2613,8 @@
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
       <c r="I24" s="8"/>
-      <c r="J24" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K24" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
       <c r="L24" s="9"/>
       <c r="M24" s="9"/>
       <c r="N24" s="9"/>
@@ -2712,12 +2647,8 @@
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
       <c r="I25" s="8"/>
-      <c r="J25" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K25" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="9"/>
       <c r="N25" s="9"/>
@@ -2750,10 +2681,10 @@
         <v>45092</v>
       </c>
       <c r="G26" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="H26" s="21" t="s">
         <v>291</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>292</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>34</v>
@@ -2769,13 +2700,13 @@
         <v>24</v>
       </c>
       <c r="N26" s="22" t="s">
+        <v>230</v>
+      </c>
+      <c r="O26" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="P26" s="22" t="s">
         <v>231</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P26" s="22" t="s">
-        <v>232</v>
       </c>
       <c r="Q26" s="22"/>
       <c r="R26" s="23"/>
@@ -2804,12 +2735,8 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
       <c r="I27" s="8"/>
-      <c r="J27" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K27" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="9"/>
       <c r="N27" s="9"/>
@@ -2833,27 +2760,23 @@
         <v>21</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>227</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8"/>
       <c r="I28" s="8"/>
-      <c r="J28" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K28" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
       <c r="L28" s="9"/>
       <c r="M28" s="9"/>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q28" s="9"/>
       <c r="R28" s="10" t="s">
@@ -2875,27 +2798,23 @@
         <v>26</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
       <c r="H29" s="8"/>
       <c r="I29" s="8"/>
-      <c r="J29" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K29" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
       <c r="L29" s="9"/>
       <c r="M29" s="9"/>
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q29" s="9"/>
       <c r="R29" s="10" t="s">
@@ -2917,27 +2836,23 @@
         <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
       <c r="H30" s="8"/>
       <c r="I30" s="8"/>
-      <c r="J30" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K30" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="9"/>
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q30" s="9"/>
       <c r="R30" s="10" t="s">
@@ -2959,27 +2874,23 @@
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
       <c r="I31" s="8"/>
-      <c r="J31" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K31" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q31" s="9"/>
       <c r="R31" s="10" t="s">
@@ -3010,12 +2921,8 @@
       <c r="G32" s="8"/>
       <c r="H32" s="8"/>
       <c r="I32" s="8"/>
-      <c r="J32" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K32" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="9"/>
       <c r="N32" s="9"/>
@@ -3048,12 +2955,8 @@
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
       <c r="I33" s="8"/>
-      <c r="J33" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K33" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J33" s="9"/>
+      <c r="K33" s="9"/>
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
       <c r="N33" s="9"/>
@@ -3086,12 +2989,8 @@
       <c r="G34" s="8"/>
       <c r="H34" s="8"/>
       <c r="I34" s="8"/>
-      <c r="J34" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K34" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J34" s="9"/>
+      <c r="K34" s="9"/>
       <c r="L34" s="9"/>
       <c r="M34" s="9"/>
       <c r="N34" s="9"/>
@@ -3124,12 +3023,8 @@
       <c r="G35" s="8"/>
       <c r="H35" s="13"/>
       <c r="I35" s="8"/>
-      <c r="J35" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K35" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
       <c r="L35" s="9"/>
       <c r="M35" s="9"/>
       <c r="N35" s="9"/>
@@ -3162,12 +3057,8 @@
       <c r="G36" s="8"/>
       <c r="H36" s="8"/>
       <c r="I36" s="8"/>
-      <c r="J36" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
       <c r="L36" s="9"/>
       <c r="M36" s="9"/>
       <c r="N36" s="9"/>
@@ -3200,12 +3091,8 @@
       <c r="G37" s="8"/>
       <c r="H37" s="8"/>
       <c r="I37" s="8"/>
-      <c r="J37" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K37" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J37" s="9"/>
+      <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="9"/>
       <c r="N37" s="9"/>
@@ -3238,12 +3125,8 @@
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
       <c r="I38" s="8"/>
-      <c r="J38" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K38" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="9"/>
       <c r="N38" s="9"/>
@@ -3276,12 +3159,8 @@
       <c r="G39" s="8"/>
       <c r="H39" s="8"/>
       <c r="I39" s="8"/>
-      <c r="J39" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K39" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J39" s="9"/>
+      <c r="K39" s="9"/>
       <c r="L39" s="9"/>
       <c r="M39" s="9"/>
       <c r="N39" s="9"/>
@@ -3305,21 +3184,17 @@
         <v>21</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>164</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>165</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
       <c r="H40" s="8"/>
       <c r="I40" s="8"/>
-      <c r="J40" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K40" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="9"/>
       <c r="N40" s="9"/>
@@ -3343,21 +3218,17 @@
         <v>21</v>
       </c>
       <c r="D41" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>166</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>167</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
       <c r="H41" s="8"/>
       <c r="I41" s="8"/>
-      <c r="J41" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K41" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
       <c r="N41" s="9"/>
@@ -3381,21 +3252,17 @@
         <v>21</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>169</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
       <c r="H42" s="8"/>
       <c r="I42" s="8"/>
-      <c r="J42" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K42" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J42" s="9"/>
+      <c r="K42" s="9"/>
       <c r="L42" s="9"/>
       <c r="M42" s="9"/>
       <c r="N42" s="9"/>
@@ -3419,21 +3286,17 @@
         <v>21</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>170</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>171</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
       <c r="H43" s="8"/>
       <c r="I43" s="8"/>
-      <c r="J43" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K43" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="9"/>
       <c r="N43" s="9"/>
@@ -3466,12 +3329,8 @@
       <c r="G44" s="8"/>
       <c r="H44" s="8"/>
       <c r="I44" s="8"/>
-      <c r="J44" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K44" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="9"/>
       <c r="N44" s="9"/>
@@ -3504,12 +3363,8 @@
       <c r="G45" s="8"/>
       <c r="H45" s="8"/>
       <c r="I45" s="8"/>
-      <c r="J45" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K45" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J45" s="9"/>
+      <c r="K45" s="9"/>
       <c r="L45" s="9"/>
       <c r="M45" s="9"/>
       <c r="N45" s="9"/>
@@ -3542,12 +3397,8 @@
       <c r="G46" s="8"/>
       <c r="H46" s="8"/>
       <c r="I46" s="8"/>
-      <c r="J46" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K46" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="9"/>
       <c r="N46" s="9"/>
@@ -3580,12 +3431,8 @@
       <c r="G47" s="8"/>
       <c r="H47" s="8"/>
       <c r="I47" s="8"/>
-      <c r="J47" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K47" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="9"/>
       <c r="N47" s="9"/>
@@ -3618,12 +3465,8 @@
       <c r="G48" s="8"/>
       <c r="H48" s="8"/>
       <c r="I48" s="8"/>
-      <c r="J48" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K48" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
       <c r="L48" s="9"/>
       <c r="M48" s="9"/>
       <c r="N48" s="9"/>
@@ -3656,12 +3499,8 @@
       <c r="G49" s="8"/>
       <c r="H49" s="8"/>
       <c r="I49" s="8"/>
-      <c r="J49" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K49" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
       <c r="L49" s="9"/>
       <c r="M49" s="9"/>
       <c r="N49" s="9"/>
@@ -3694,12 +3533,8 @@
       <c r="G50" s="8"/>
       <c r="H50" s="8"/>
       <c r="I50" s="8"/>
-      <c r="J50" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K50" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
       <c r="L50" s="9"/>
       <c r="M50" s="9"/>
       <c r="N50" s="9"/>
@@ -3723,21 +3558,17 @@
         <v>26</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>172</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>173</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
       <c r="H51" s="8"/>
       <c r="I51" s="8"/>
-      <c r="J51" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K51" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
       <c r="N51" s="9"/>
@@ -3770,12 +3601,8 @@
       <c r="G52" s="8"/>
       <c r="H52" s="8"/>
       <c r="I52" s="8"/>
-      <c r="J52" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K52" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
       <c r="L52" s="9"/>
       <c r="M52" s="9"/>
       <c r="N52" s="9"/>
@@ -3808,12 +3635,8 @@
       <c r="G53" s="8"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
-      <c r="J53" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K53" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
       <c r="L53" s="9"/>
       <c r="M53" s="9"/>
       <c r="N53" s="9"/>
@@ -3846,12 +3669,8 @@
       <c r="G54" s="8"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
-      <c r="J54" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K54" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
       <c r="L54" s="9"/>
       <c r="M54" s="9"/>
       <c r="N54" s="9"/>
@@ -3875,21 +3694,17 @@
         <v>26</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>174</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>175</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
       <c r="H55" s="8"/>
       <c r="I55" s="8"/>
-      <c r="J55" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K55" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
       <c r="L55" s="9"/>
       <c r="M55" s="9"/>
       <c r="N55" s="9"/>
@@ -3913,21 +3728,17 @@
         <v>26</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>176</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>177</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
       <c r="H56" s="8"/>
       <c r="I56" s="8"/>
-      <c r="J56" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K56" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
       <c r="L56" s="9"/>
       <c r="M56" s="9"/>
       <c r="N56" s="9"/>
@@ -3951,21 +3762,17 @@
         <v>26</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>178</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>179</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
       <c r="H57" s="8"/>
       <c r="I57" s="8"/>
-      <c r="J57" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K57" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
       <c r="L57" s="9"/>
       <c r="M57" s="9"/>
       <c r="N57" s="9"/>
@@ -3989,21 +3796,17 @@
         <v>26</v>
       </c>
       <c r="D58" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>180</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>181</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
       <c r="H58" s="8"/>
       <c r="I58" s="8"/>
-      <c r="J58" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K58" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
       <c r="L58" s="9"/>
       <c r="M58" s="9"/>
       <c r="N58" s="9"/>
@@ -4027,21 +3830,17 @@
         <v>26</v>
       </c>
       <c r="D59" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>182</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>183</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
       <c r="H59" s="8"/>
       <c r="I59" s="8"/>
-      <c r="J59" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K59" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
       <c r="L59" s="9"/>
       <c r="M59" s="9"/>
       <c r="N59" s="9"/>
@@ -4065,21 +3864,17 @@
         <v>26</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>184</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>185</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
       <c r="H60" s="8"/>
       <c r="I60" s="8"/>
-      <c r="J60" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K60" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
       <c r="L60" s="9"/>
       <c r="M60" s="9"/>
       <c r="N60" s="9"/>
@@ -4103,21 +3898,17 @@
         <v>26</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
       <c r="H61" s="8"/>
       <c r="I61" s="8"/>
-      <c r="J61" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K61" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J61" s="9"/>
+      <c r="K61" s="9"/>
       <c r="L61" s="9"/>
       <c r="M61" s="9"/>
       <c r="N61" s="9"/>
@@ -4141,21 +3932,17 @@
         <v>26</v>
       </c>
       <c r="D62" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>188</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>189</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
       <c r="H62" s="8"/>
       <c r="I62" s="8"/>
-      <c r="J62" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K62" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
       <c r="L62" s="9"/>
       <c r="M62" s="9"/>
       <c r="N62" s="9"/>
@@ -4188,12 +3975,8 @@
       <c r="G63" s="8"/>
       <c r="H63" s="8"/>
       <c r="I63" s="8"/>
-      <c r="J63" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K63" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J63" s="9"/>
+      <c r="K63" s="9"/>
       <c r="L63" s="9"/>
       <c r="M63" s="9"/>
       <c r="N63" s="9"/>
@@ -4226,12 +4009,8 @@
       <c r="G64" s="8"/>
       <c r="H64" s="8"/>
       <c r="I64" s="8"/>
-      <c r="J64" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K64" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
       <c r="L64" s="9"/>
       <c r="M64" s="9"/>
       <c r="N64" s="9"/>
@@ -4264,12 +4043,8 @@
       <c r="G65" s="8"/>
       <c r="H65" s="8"/>
       <c r="I65" s="8"/>
-      <c r="J65" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K65" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
       <c r="L65" s="9"/>
       <c r="M65" s="9"/>
       <c r="N65" s="9"/>
@@ -4302,12 +4077,8 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
       <c r="I66" s="8"/>
-      <c r="J66" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K66" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J66" s="9"/>
+      <c r="K66" s="9"/>
       <c r="L66" s="9"/>
       <c r="M66" s="9"/>
       <c r="N66" s="9"/>
@@ -4340,12 +4111,8 @@
       <c r="G67" s="8"/>
       <c r="H67" s="13"/>
       <c r="I67" s="8"/>
-      <c r="J67" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K67" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J67" s="9"/>
+      <c r="K67" s="9"/>
       <c r="L67" s="9"/>
       <c r="M67" s="9"/>
       <c r="N67" s="9"/>
@@ -4378,12 +4145,8 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8"/>
       <c r="I68" s="8"/>
-      <c r="J68" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K68" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
       <c r="L68" s="9"/>
       <c r="M68" s="9"/>
       <c r="N68" s="9"/>
@@ -4416,12 +4179,8 @@
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
       <c r="I69" s="8"/>
-      <c r="J69" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K69" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J69" s="9"/>
+      <c r="K69" s="9"/>
       <c r="L69" s="9"/>
       <c r="M69" s="9"/>
       <c r="N69" s="9"/>
@@ -4454,12 +4213,8 @@
       <c r="G70" s="8"/>
       <c r="H70" s="8"/>
       <c r="I70" s="8"/>
-      <c r="J70" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K70" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
       <c r="L70" s="9"/>
       <c r="M70" s="9"/>
       <c r="N70" s="9"/>
@@ -4492,12 +4247,8 @@
       <c r="G71" s="8"/>
       <c r="H71" s="8"/>
       <c r="I71" s="8"/>
-      <c r="J71" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K71" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
       <c r="L71" s="9"/>
       <c r="M71" s="9"/>
       <c r="N71" s="9"/>
@@ -4530,12 +4281,8 @@
       <c r="G72" s="8"/>
       <c r="H72" s="8"/>
       <c r="I72" s="8"/>
-      <c r="J72" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K72" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
       <c r="L72" s="9"/>
       <c r="M72" s="9"/>
       <c r="N72" s="9"/>
@@ -4568,12 +4315,8 @@
       <c r="G73" s="8"/>
       <c r="H73" s="8"/>
       <c r="I73" s="8"/>
-      <c r="J73" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K73" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
       <c r="L73" s="9"/>
       <c r="M73" s="9"/>
       <c r="N73" s="9"/>
@@ -4606,12 +4349,8 @@
       <c r="G74" s="8"/>
       <c r="H74" s="8"/>
       <c r="I74" s="8"/>
-      <c r="J74" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K74" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
       <c r="L74" s="9"/>
       <c r="M74" s="9"/>
       <c r="N74" s="9"/>
@@ -4635,21 +4374,17 @@
         <v>29</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>190</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>191</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
       <c r="H75" s="8"/>
       <c r="I75" s="8"/>
-      <c r="J75" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K75" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
       <c r="L75" s="9"/>
       <c r="M75" s="9"/>
       <c r="N75" s="9"/>
@@ -4673,21 +4408,17 @@
         <v>29</v>
       </c>
       <c r="D76" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>192</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>193</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
       <c r="H76" s="8"/>
       <c r="I76" s="8"/>
-      <c r="J76" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K76" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
       <c r="L76" s="9"/>
       <c r="M76" s="9"/>
       <c r="N76" s="9"/>
@@ -4711,21 +4442,17 @@
         <v>29</v>
       </c>
       <c r="D77" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>194</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>195</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
       <c r="H77" s="8"/>
       <c r="I77" s="8"/>
-      <c r="J77" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K77" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
       <c r="L77" s="9"/>
       <c r="M77" s="9"/>
       <c r="N77" s="9"/>
@@ -4758,12 +4485,8 @@
       <c r="G78" s="8"/>
       <c r="H78" s="8"/>
       <c r="I78" s="8"/>
-      <c r="J78" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K78" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
       <c r="L78" s="9"/>
       <c r="M78" s="9"/>
       <c r="N78" s="9"/>
@@ -4787,21 +4510,17 @@
         <v>29</v>
       </c>
       <c r="D79" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>196</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>197</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
       <c r="H79" s="8"/>
       <c r="I79" s="8"/>
-      <c r="J79" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K79" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
       <c r="L79" s="9"/>
       <c r="M79" s="9"/>
       <c r="N79" s="9"/>
@@ -4834,12 +4553,8 @@
       <c r="G80" s="8"/>
       <c r="H80" s="8"/>
       <c r="I80" s="8"/>
-      <c r="J80" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K80" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
       <c r="L80" s="9"/>
       <c r="M80" s="9"/>
       <c r="N80" s="9"/>
@@ -4872,12 +4587,8 @@
       <c r="G81" s="8"/>
       <c r="H81" s="8"/>
       <c r="I81" s="8"/>
-      <c r="J81" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K81" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J81" s="9"/>
+      <c r="K81" s="9"/>
       <c r="L81" s="9"/>
       <c r="M81" s="9"/>
       <c r="N81" s="9"/>
@@ -4901,21 +4612,17 @@
         <v>29</v>
       </c>
       <c r="D82" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>198</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>199</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
       <c r="H82" s="8"/>
       <c r="I82" s="8"/>
-      <c r="J82" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K82" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
       <c r="L82" s="9"/>
       <c r="M82" s="9"/>
       <c r="N82" s="9"/>
@@ -4948,12 +4655,8 @@
       <c r="G83" s="8"/>
       <c r="H83" s="8"/>
       <c r="I83" s="8"/>
-      <c r="J83" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K83" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J83" s="9"/>
+      <c r="K83" s="9"/>
       <c r="L83" s="9"/>
       <c r="M83" s="9"/>
       <c r="N83" s="9"/>
@@ -4986,12 +4689,8 @@
       <c r="G84" s="8"/>
       <c r="H84" s="8"/>
       <c r="I84" s="8"/>
-      <c r="J84" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K84" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
       <c r="L84" s="9"/>
       <c r="M84" s="9"/>
       <c r="N84" s="9"/>
@@ -5024,12 +4723,8 @@
       <c r="G85" s="8"/>
       <c r="H85" s="8"/>
       <c r="I85" s="8"/>
-      <c r="J85" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K85" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
       <c r="L85" s="9"/>
       <c r="M85" s="9"/>
       <c r="N85" s="9"/>
@@ -5053,21 +4748,17 @@
         <v>29</v>
       </c>
       <c r="D86" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="E86" s="6" t="s">
         <v>200</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>201</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
       <c r="H86" s="8"/>
       <c r="I86" s="8"/>
-      <c r="J86" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K86" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J86" s="9"/>
+      <c r="K86" s="9"/>
       <c r="L86" s="9"/>
       <c r="M86" s="9"/>
       <c r="N86" s="9"/>
@@ -5091,21 +4782,17 @@
         <v>29</v>
       </c>
       <c r="D87" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="E87" s="6" t="s">
         <v>202</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>203</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
       <c r="H87" s="8"/>
       <c r="I87" s="8"/>
-      <c r="J87" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K87" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
       <c r="L87" s="9"/>
       <c r="M87" s="9"/>
       <c r="N87" s="9"/>
@@ -5138,13 +4825,13 @@
         <v>45055</v>
       </c>
       <c r="G88" s="21" t="s">
+        <v>236</v>
+      </c>
+      <c r="H88" s="21" t="s">
         <v>237</v>
       </c>
-      <c r="H88" s="21" t="s">
+      <c r="I88" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="I88" s="21" t="s">
-        <v>239</v>
       </c>
       <c r="J88" s="22" t="s">
         <v>24</v>
@@ -5173,22 +4860,22 @@
         <v>37</v>
       </c>
       <c r="D89" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E89" s="19" t="s">
         <v>204</v>
-      </c>
-      <c r="E89" s="19" t="s">
-        <v>205</v>
       </c>
       <c r="F89" s="20">
         <v>45058</v>
       </c>
       <c r="G89" s="21" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H89" s="21" t="s">
+        <v>237</v>
+      </c>
+      <c r="I89" s="21" t="s">
         <v>238</v>
-      </c>
-      <c r="I89" s="21" t="s">
-        <v>239</v>
       </c>
       <c r="J89" s="27" t="s">
         <v>24</v>
@@ -5217,28 +4904,28 @@
         <v>37</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>206</v>
-      </c>
-      <c r="E90" s="6" t="s">
-        <v>207</v>
       </c>
       <c r="F90" s="7">
         <v>45058</v>
       </c>
       <c r="G90" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="H90" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="H90" s="8" t="s">
+      <c r="I90" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="I90" s="8" t="s">
-        <v>242</v>
-      </c>
       <c r="J90" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K90" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
@@ -5263,28 +4950,28 @@
         <v>37</v>
       </c>
       <c r="D91" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>208</v>
-      </c>
-      <c r="E91" s="6" t="s">
-        <v>209</v>
       </c>
       <c r="F91" s="7">
         <v>45058</v>
       </c>
       <c r="G91" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="H91" s="8" t="s">
         <v>243</v>
       </c>
-      <c r="H91" s="8" t="s">
+      <c r="I91" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="I91" s="8" t="s">
-        <v>245</v>
-      </c>
       <c r="J91" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K91" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
@@ -5318,13 +5005,13 @@
         <v>45058</v>
       </c>
       <c r="G92" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="H92" s="8" t="s">
         <v>246</v>
       </c>
-      <c r="H92" s="8" t="s">
+      <c r="I92" s="8" t="s">
         <v>247</v>
-      </c>
-      <c r="I92" s="8" t="s">
-        <v>248</v>
       </c>
       <c r="J92" s="9" t="s">
         <v>24</v>
@@ -5337,13 +5024,13 @@
         <v>24</v>
       </c>
       <c r="N92" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O92" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P92" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O92" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P92" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q92" s="9"/>
       <c r="R92" s="10"/>
@@ -5372,13 +5059,13 @@
         <v>45058</v>
       </c>
       <c r="G93" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="H93" s="8" t="s">
         <v>249</v>
       </c>
-      <c r="H93" s="8" t="s">
+      <c r="I93" s="8" t="s">
         <v>250</v>
-      </c>
-      <c r="I93" s="8" t="s">
-        <v>251</v>
       </c>
       <c r="J93" s="9" t="s">
         <v>24</v>
@@ -5391,13 +5078,13 @@
         <v>24</v>
       </c>
       <c r="N93" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O93" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P93" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O93" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P93" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q93" s="9"/>
       <c r="R93" s="10"/>
@@ -5426,13 +5113,13 @@
         <v>45058</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H94" s="8" t="s">
         <v>125</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="J94" s="9" t="s">
         <v>24</v>
@@ -5445,13 +5132,13 @@
         <v>24</v>
       </c>
       <c r="N94" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O94" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P94" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O94" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P94" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q94" s="9"/>
       <c r="R94" s="10"/>
@@ -5480,13 +5167,13 @@
         <v>45058</v>
       </c>
       <c r="G95" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="H95" s="8" t="s">
         <v>254</v>
       </c>
-      <c r="H95" s="8" t="s">
+      <c r="I95" s="8" t="s">
         <v>255</v>
-      </c>
-      <c r="I95" s="8" t="s">
-        <v>256</v>
       </c>
       <c r="J95" s="9" t="s">
         <v>24</v>
@@ -5499,13 +5186,13 @@
         <v>24</v>
       </c>
       <c r="N95" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O95" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P95" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O95" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P95" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q95" s="9"/>
       <c r="R95" s="10"/>
@@ -5534,13 +5221,13 @@
         <v>45058</v>
       </c>
       <c r="G96" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="H96" s="8" t="s">
         <v>257</v>
       </c>
-      <c r="H96" s="8" t="s">
+      <c r="I96" s="8" t="s">
         <v>258</v>
-      </c>
-      <c r="I96" s="8" t="s">
-        <v>259</v>
       </c>
       <c r="J96" s="9" t="s">
         <v>24</v>
@@ -5553,13 +5240,13 @@
         <v>24</v>
       </c>
       <c r="N96" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O96" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P96" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O96" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P96" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q96" s="9"/>
       <c r="R96" s="10"/>
@@ -5588,13 +5275,13 @@
         <v>45058</v>
       </c>
       <c r="G97" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="H97" s="8" t="s">
         <v>260</v>
       </c>
-      <c r="H97" s="8" t="s">
+      <c r="I97" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="I97" s="8" t="s">
-        <v>262</v>
       </c>
       <c r="J97" s="9" t="s">
         <v>24</v>
@@ -5607,13 +5294,13 @@
         <v>24</v>
       </c>
       <c r="N97" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O97" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P97" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O97" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P97" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q97" s="9"/>
       <c r="R97" s="10"/>
@@ -5633,41 +5320,41 @@
         <v>37</v>
       </c>
       <c r="D98" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="E98" s="6" t="s">
         <v>210</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>211</v>
       </c>
       <c r="F98" s="7">
         <v>45058</v>
       </c>
       <c r="G98" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="H98" s="8" t="s">
         <v>263</v>
       </c>
-      <c r="H98" s="8" t="s">
+      <c r="I98" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="I98" s="8" t="s">
-        <v>265</v>
       </c>
       <c r="J98" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K98" s="9"/>
       <c r="L98" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M98" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N98" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O98" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="P98" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O98" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="P98" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q98" s="9"/>
       <c r="R98" s="10"/>
@@ -5687,41 +5374,41 @@
         <v>37</v>
       </c>
       <c r="D99" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E99" s="6" t="s">
         <v>212</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>213</v>
       </c>
       <c r="F99" s="7">
         <v>45058</v>
       </c>
       <c r="G99" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="H99" s="8" t="s">
         <v>266</v>
       </c>
-      <c r="H99" s="8" t="s">
+      <c r="I99" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="I99" s="8" t="s">
-        <v>268</v>
       </c>
       <c r="J99" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K99" s="9"/>
       <c r="L99" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="M99" s="9" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="N99" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O99" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="P99" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O99" s="9" t="s">
-        <v>288</v>
-      </c>
-      <c r="P99" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q99" s="9"/>
       <c r="R99" s="10"/>
@@ -5750,13 +5437,13 @@
         <v>45058</v>
       </c>
       <c r="G100" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="H100" s="8" t="s">
         <v>269</v>
       </c>
-      <c r="H100" s="8" t="s">
+      <c r="I100" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="I100" s="8" t="s">
-        <v>271</v>
       </c>
       <c r="J100" s="9" t="s">
         <v>24</v>
@@ -5769,13 +5456,13 @@
         <v>24</v>
       </c>
       <c r="N100" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O100" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P100" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O100" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P100" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q100" s="9"/>
       <c r="R100" s="10"/>
@@ -5804,13 +5491,13 @@
         <v>45058</v>
       </c>
       <c r="G101" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="H101" s="8" t="s">
         <v>272</v>
       </c>
-      <c r="H101" s="8" t="s">
+      <c r="I101" s="8" t="s">
         <v>273</v>
-      </c>
-      <c r="I101" s="8" t="s">
-        <v>274</v>
       </c>
       <c r="J101" s="9" t="s">
         <v>24</v>
@@ -5823,13 +5510,13 @@
         <v>24</v>
       </c>
       <c r="N101" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O101" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P101" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O101" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P101" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q101" s="9"/>
       <c r="R101" s="10"/>
@@ -5858,13 +5545,13 @@
         <v>45058</v>
       </c>
       <c r="G102" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="H102" s="8" t="s">
         <v>275</v>
       </c>
-      <c r="H102" s="8" t="s">
+      <c r="I102" s="8" t="s">
         <v>276</v>
-      </c>
-      <c r="I102" s="8" t="s">
-        <v>277</v>
       </c>
       <c r="J102" s="9" t="s">
         <v>24</v>
@@ -5877,13 +5564,13 @@
         <v>24</v>
       </c>
       <c r="N102" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O102" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P102" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O102" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P102" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q102" s="9"/>
       <c r="R102" s="10"/>
@@ -5903,22 +5590,22 @@
         <v>37</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="E103" s="6" t="s">
         <v>214</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>215</v>
       </c>
       <c r="F103" s="7">
         <v>45058</v>
       </c>
       <c r="G103" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="H103" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="H103" s="8" t="s">
+      <c r="I103" s="8" t="s">
         <v>279</v>
-      </c>
-      <c r="I103" s="8" t="s">
-        <v>280</v>
       </c>
       <c r="J103" s="9" t="s">
         <v>24</v>
@@ -5931,13 +5618,13 @@
         <v>24</v>
       </c>
       <c r="N103" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O103" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P103" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O103" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P103" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q103" s="9"/>
       <c r="R103" s="10"/>
@@ -5966,13 +5653,13 @@
         <v>45058</v>
       </c>
       <c r="G104" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H104" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="H104" s="8" t="s">
+      <c r="I104" s="8" t="s">
         <v>282</v>
-      </c>
-      <c r="I104" s="8" t="s">
-        <v>283</v>
       </c>
       <c r="J104" s="9" t="s">
         <v>24</v>
@@ -5985,13 +5672,13 @@
         <v>24</v>
       </c>
       <c r="N104" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O104" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P104" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O104" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P104" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q104" s="9"/>
       <c r="R104" s="10"/>
@@ -6011,21 +5698,17 @@
         <v>37</v>
       </c>
       <c r="D105" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="E105" s="6" t="s">
         <v>216</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>217</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
       <c r="H105" s="8"/>
       <c r="I105" s="8"/>
-      <c r="J105" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K105" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
       <c r="N105" s="9"/>
@@ -6049,21 +5732,17 @@
         <v>37</v>
       </c>
       <c r="D106" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="E106" s="6" t="s">
         <v>218</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>219</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
       <c r="H106" s="8"/>
       <c r="I106" s="8"/>
-      <c r="J106" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K106" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
       <c r="L106" s="9"/>
       <c r="M106" s="9"/>
       <c r="N106" s="9"/>
@@ -6087,21 +5766,17 @@
         <v>37</v>
       </c>
       <c r="D107" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="E107" s="6" t="s">
         <v>220</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>221</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
       <c r="H107" s="8"/>
       <c r="I107" s="8"/>
-      <c r="J107" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K107" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
       <c r="L107" s="9"/>
       <c r="M107" s="9"/>
       <c r="N107" s="9"/>
@@ -6125,21 +5800,17 @@
         <v>37</v>
       </c>
       <c r="D108" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="E108" s="6" t="s">
         <v>222</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>223</v>
       </c>
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
-      <c r="J108" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K108" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
       <c r="L108" s="9"/>
       <c r="M108" s="9"/>
       <c r="N108" s="9"/>
@@ -6163,21 +5834,17 @@
         <v>37</v>
       </c>
       <c r="D109" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="E109" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>225</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
       <c r="H109" s="8"/>
       <c r="I109" s="8"/>
-      <c r="J109" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="K109" s="9" t="s">
-        <v>293</v>
-      </c>
+      <c r="J109" s="9"/>
+      <c r="K109" s="9"/>
       <c r="L109" s="9"/>
       <c r="M109" s="9"/>
       <c r="N109" s="9"/>
@@ -6210,13 +5877,13 @@
         <v>45058</v>
       </c>
       <c r="G110" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="H110" s="8" t="s">
         <v>284</v>
       </c>
-      <c r="H110" s="8" t="s">
+      <c r="I110" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="I110" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="J110" s="9" t="s">
         <v>24</v>
@@ -6229,13 +5896,13 @@
         <v>24</v>
       </c>
       <c r="N110" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="O110" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P110" s="9" t="s">
         <v>231</v>
-      </c>
-      <c r="O110" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P110" s="9" t="s">
-        <v>232</v>
       </c>
       <c r="Q110" s="9"/>
       <c r="R110" s="10"/>

</xml_diff>

<commit_message>
Aggiornato data.json e report-chekclist
S1#111EUROMEDICAL
EUROMEDICAL
MEDIWEB
1.0
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111EUROMEDICAL/EUROMEDICAL/MEDIWEB/1.0/report-checklist.xlsx
+++ b/GATEWAY/S1#111EUROMEDICAL/EUROMEDICAL/MEDIWEB/1.0/report-checklist.xlsx
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="721" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="288">
   <si>
     <t>ID</t>
   </si>
@@ -688,9 +688,6 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>Le informazioni logicamente afferenti alle sezioni opzionali richieste nel test sono incluse in modo non strutturato nella sezione "Referto".</t>
-  </si>
-  <si>
     <t>VALIDAZIONE_CDA2_RAD_CT3</t>
   </si>
   <si>
@@ -1055,30 +1052,9 @@
     <t>2023-05-09T10:31:04Z</t>
   </si>
   <si>
-    <t>11dd9d6006dd296b</t>
-  </si>
-  <si>
     <t>2.16.840.1.113883.2.9.2.120.4.4.2f4f313cb2e0ce8e818e774cb40980b61a0afdaa6c3d9b9c9bde5816b4a76f34.d079c92dfa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-05-12T14:57:30Z</t>
-  </si>
-  <si>
-    <t>a6e84cfd5ae7aa23</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2f4f313cb2e0ce8e818e774cb40980b61a0afdaa6c3d9b9c9bde5816b4a76f34.3b969b6aa8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-05-12T15:10:09Z</t>
-  </si>
-  <si>
-    <t>b5032a90e4700c0c</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.120.4.4.2f4f313cb2e0ce8e818e774cb40980b61a0afdaa6c3d9b9c9bde5816b4a76f34.06279f2b69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-05-12T15:18:30Z</t>
   </si>
   <si>
@@ -1202,24 +1178,9 @@
     <t>2.16.840.1.113883.2.9.2.120.4.4.2f4f313cb2e0ce8e818e774cb40980b61a0afdaa6c3d9b9c9bde5816b4a76f34.84900737e0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-05-12T14:46:11Z</t>
-  </si>
-  <si>
     <t>Si</t>
   </si>
   <si>
-    <t>2023-06-15T08:45:58Z</t>
-  </si>
-  <si>
-    <t>39ca4090e01f3d61</t>
-  </si>
-  <si>
-    <t>2023-06-15T08:50:08Z</t>
-  </si>
-  <si>
-    <t>f1b6258b62dda099</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -1227,13 +1188,31 @@
   </si>
   <si>
     <t>Non gestito</t>
+  </si>
+  <si>
+    <t>5ef067ff5db57808</t>
+  </si>
+  <si>
+    <t>Applicativo non gestisce alcune sezioni opzionali</t>
+  </si>
+  <si>
+    <t>2ec8a1d3fee31b96</t>
+  </si>
+  <si>
+    <t>2023-06-27T09:30:55Z</t>
+  </si>
+  <si>
+    <t>af572281ebe37c01</t>
+  </si>
+  <si>
+    <t>2023-06-27T09:36:10Z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1298,12 +1277,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1588,12 +1561,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="1"/>
     </xf>
@@ -1619,6 +1586,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -1903,10 +1876,10 @@
   <dimension ref="A1:T111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="46" zoomScaleNormal="46" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="E107" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="D102" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K108" sqref="K108"/>
+      <selection pane="bottomRight" activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1930,44 +1903,44 @@
       <c r="C1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="31" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="D2" s="30"/>
+    </row>
+    <row r="3" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="35"/>
+      <c r="C3" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="D2" s="32"/>
-    </row>
-    <row r="3" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="36" t="s">
-        <v>143</v>
-      </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="35" t="s">
+      <c r="D3" s="28"/>
+    </row>
+    <row r="4" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="36"/>
+      <c r="B4" s="37"/>
+      <c r="C4" s="33" t="s">
         <v>233</v>
       </c>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="38"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="35" t="s">
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="38"/>
+      <c r="B5" s="39"/>
+      <c r="C5" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="D4" s="30"/>
-    </row>
-    <row r="5" spans="1:20" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="35" t="s">
-        <v>235</v>
-      </c>
-      <c r="D5" s="30"/>
+      <c r="D5" s="28"/>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="31"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="16"/>
     </row>
     <row r="7" spans="1:20" ht="37.5" thickBot="1" x14ac:dyDescent="0.4">
@@ -2053,7 +2026,7 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9" t="s">
-        <v>292</v>
+        <v>279</v>
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
@@ -2249,10 +2222,10 @@
         <v>26</v>
       </c>
       <c r="D14" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>153</v>
-      </c>
-      <c r="E14" s="6" t="s">
-        <v>154</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8"/>
@@ -2283,10 +2256,10 @@
         <v>26</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>155</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>156</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
@@ -2351,10 +2324,10 @@
         <v>29</v>
       </c>
       <c r="D17" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="E17" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="E17" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8"/>
@@ -2385,10 +2358,10 @@
         <v>29</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>159</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>160</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8"/>
@@ -2419,10 +2392,10 @@
         <v>29</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="E19" s="6" t="s">
         <v>161</v>
-      </c>
-      <c r="E19" s="6" t="s">
-        <v>162</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8"/>
@@ -2503,7 +2476,7 @@
       <c r="N21" s="9"/>
       <c r="O21" s="9"/>
       <c r="P21" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q21" s="9"/>
       <c r="R21" s="10"/>
@@ -2529,13 +2502,13 @@
         <v>33</v>
       </c>
       <c r="F22" s="20">
-        <v>45092</v>
+        <v>45104</v>
       </c>
       <c r="G22" s="21" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="I22" s="21" t="s">
         <v>34</v>
@@ -2551,13 +2524,13 @@
         <v>24</v>
       </c>
       <c r="N22" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="O22" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="P22" s="22" t="s">
         <v>230</v>
-      </c>
-      <c r="O22" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P22" s="22" t="s">
-        <v>231</v>
       </c>
       <c r="Q22" s="22"/>
       <c r="R22" s="23"/>
@@ -2685,13 +2658,13 @@
         <v>41</v>
       </c>
       <c r="F26" s="20">
-        <v>45092</v>
+        <v>45104</v>
       </c>
       <c r="G26" s="21" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="H26" s="21" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="I26" s="21" t="s">
         <v>34</v>
@@ -2707,13 +2680,13 @@
         <v>24</v>
       </c>
       <c r="N26" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="O26" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="P26" s="22" t="s">
         <v>230</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P26" s="22" t="s">
-        <v>231</v>
       </c>
       <c r="Q26" s="22"/>
       <c r="R26" s="23"/>
@@ -2767,10 +2740,10 @@
         <v>21</v>
       </c>
       <c r="D28" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="E28" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>226</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8"/>
@@ -2801,10 +2774,10 @@
         <v>26</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8"/>
@@ -2817,7 +2790,7 @@
       <c r="N29" s="9"/>
       <c r="O29" s="9"/>
       <c r="P29" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q29" s="9"/>
       <c r="R29" s="10" t="s">
@@ -2839,10 +2812,10 @@
         <v>37</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8"/>
@@ -2855,7 +2828,7 @@
       <c r="N30" s="9"/>
       <c r="O30" s="9"/>
       <c r="P30" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q30" s="9"/>
       <c r="R30" s="10" t="s">
@@ -2877,10 +2850,10 @@
         <v>29</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8"/>
@@ -2893,7 +2866,7 @@
       <c r="N31" s="9"/>
       <c r="O31" s="9"/>
       <c r="P31" s="9" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="Q31" s="9"/>
       <c r="R31" s="10" t="s">
@@ -3187,10 +3160,10 @@
         <v>21</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="E40" s="6" t="s">
         <v>163</v>
-      </c>
-      <c r="E40" s="6" t="s">
-        <v>164</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8"/>
@@ -3221,10 +3194,10 @@
         <v>21</v>
       </c>
       <c r="D41" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="E41" s="6" t="s">
-        <v>166</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8"/>
@@ -3255,10 +3228,10 @@
         <v>21</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" s="6" t="s">
         <v>167</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="8"/>
@@ -3289,10 +3262,10 @@
         <v>21</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="E43" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="E43" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8"/>
@@ -3561,10 +3534,10 @@
         <v>26</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="E51" s="6" t="s">
         <v>171</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>172</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8"/>
@@ -3697,10 +3670,10 @@
         <v>26</v>
       </c>
       <c r="D55" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E55" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="E55" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="F55" s="7"/>
       <c r="G55" s="8"/>
@@ -3731,10 +3704,10 @@
         <v>26</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="E56" s="6" t="s">
         <v>175</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>176</v>
       </c>
       <c r="F56" s="7"/>
       <c r="G56" s="8"/>
@@ -3765,10 +3738,10 @@
         <v>26</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E57" s="6" t="s">
         <v>177</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>178</v>
       </c>
       <c r="F57" s="7"/>
       <c r="G57" s="8"/>
@@ -3799,10 +3772,10 @@
         <v>26</v>
       </c>
       <c r="D58" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="E58" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="F58" s="7"/>
       <c r="G58" s="8"/>
@@ -3833,10 +3806,10 @@
         <v>26</v>
       </c>
       <c r="D59" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="E59" s="6" t="s">
         <v>181</v>
-      </c>
-      <c r="E59" s="6" t="s">
-        <v>182</v>
       </c>
       <c r="F59" s="7"/>
       <c r="G59" s="8"/>
@@ -3867,10 +3840,10 @@
         <v>26</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="E60" s="6" t="s">
         <v>183</v>
-      </c>
-      <c r="E60" s="6" t="s">
-        <v>184</v>
       </c>
       <c r="F60" s="7"/>
       <c r="G60" s="8"/>
@@ -3901,10 +3874,10 @@
         <v>26</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="E61" s="6" t="s">
         <v>185</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>186</v>
       </c>
       <c r="F61" s="7"/>
       <c r="G61" s="8"/>
@@ -3935,10 +3908,10 @@
         <v>26</v>
       </c>
       <c r="D62" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="E62" s="6" t="s">
         <v>187</v>
-      </c>
-      <c r="E62" s="6" t="s">
-        <v>188</v>
       </c>
       <c r="F62" s="7"/>
       <c r="G62" s="8"/>
@@ -4377,10 +4350,10 @@
         <v>29</v>
       </c>
       <c r="D75" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="E75" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="F75" s="7"/>
       <c r="G75" s="8"/>
@@ -4411,10 +4384,10 @@
         <v>29</v>
       </c>
       <c r="D76" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>191</v>
-      </c>
-      <c r="E76" s="6" t="s">
-        <v>192</v>
       </c>
       <c r="F76" s="7"/>
       <c r="G76" s="8"/>
@@ -4445,10 +4418,10 @@
         <v>29</v>
       </c>
       <c r="D77" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="E77" s="6" t="s">
         <v>193</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>194</v>
       </c>
       <c r="F77" s="7"/>
       <c r="G77" s="8"/>
@@ -4513,10 +4486,10 @@
         <v>29</v>
       </c>
       <c r="D79" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="E79" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="F79" s="7"/>
       <c r="G79" s="8"/>
@@ -4615,10 +4588,10 @@
         <v>29</v>
       </c>
       <c r="D82" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="E82" s="6" t="s">
         <v>197</v>
-      </c>
-      <c r="E82" s="6" t="s">
-        <v>198</v>
       </c>
       <c r="F82" s="7"/>
       <c r="G82" s="8"/>
@@ -4751,10 +4724,10 @@
         <v>29</v>
       </c>
       <c r="D86" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="E86" s="6" t="s">
         <v>199</v>
-      </c>
-      <c r="E86" s="6" t="s">
-        <v>200</v>
       </c>
       <c r="F86" s="7"/>
       <c r="G86" s="8"/>
@@ -4785,10 +4758,10 @@
         <v>29</v>
       </c>
       <c r="D87" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="E87" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="E87" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="8"/>
@@ -4828,13 +4801,13 @@
         <v>45055</v>
       </c>
       <c r="G88" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="H88" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="I88" s="21" t="s">
         <v>236</v>
-      </c>
-      <c r="H88" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="I88" s="21" t="s">
-        <v>238</v>
       </c>
       <c r="J88" s="22" t="s">
         <v>24</v>
@@ -4863,27 +4836,21 @@
         <v>37</v>
       </c>
       <c r="D89" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E89" s="19" t="s">
         <v>203</v>
       </c>
-      <c r="E89" s="19" t="s">
-        <v>204</v>
-      </c>
-      <c r="F89" s="20">
-        <v>45058</v>
-      </c>
-      <c r="G89" s="21" t="s">
-        <v>286</v>
-      </c>
-      <c r="H89" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="I89" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="J89" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="K89" s="28"/>
+      <c r="F89" s="20"/>
+      <c r="G89" s="21"/>
+      <c r="H89" s="21"/>
+      <c r="I89" s="21"/>
+      <c r="J89" s="40" t="s">
+        <v>280</v>
+      </c>
+      <c r="K89" s="41" t="s">
+        <v>283</v>
+      </c>
       <c r="L89" s="22"/>
       <c r="M89" s="22"/>
       <c r="N89" s="22"/>
@@ -4907,28 +4874,20 @@
         <v>37</v>
       </c>
       <c r="D90" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="E90" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="E90" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="F90" s="7">
-        <v>45058</v>
-      </c>
-      <c r="G90" s="8" t="s">
-        <v>239</v>
-      </c>
-      <c r="H90" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="I90" s="8" t="s">
-        <v>241</v>
-      </c>
+      <c r="F90" s="7"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
       <c r="J90" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K90" s="6" t="s">
-        <v>152</v>
+        <v>280</v>
+      </c>
+      <c r="K90" s="9" t="s">
+        <v>283</v>
       </c>
       <c r="L90" s="9"/>
       <c r="M90" s="9"/>
@@ -4953,28 +4912,20 @@
         <v>37</v>
       </c>
       <c r="D91" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="E91" s="6" t="s">
         <v>207</v>
       </c>
-      <c r="E91" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="F91" s="7">
-        <v>45058</v>
-      </c>
-      <c r="G91" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="H91" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="I91" s="8" t="s">
-        <v>244</v>
-      </c>
+      <c r="F91" s="7"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
       <c r="J91" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="K91" s="6" t="s">
-        <v>152</v>
+        <v>280</v>
+      </c>
+      <c r="K91" s="9" t="s">
+        <v>283</v>
       </c>
       <c r="L91" s="9"/>
       <c r="M91" s="9"/>
@@ -5008,13 +4959,13 @@
         <v>45058</v>
       </c>
       <c r="G92" s="8" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="H92" s="8" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="I92" s="8" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="J92" s="9" t="s">
         <v>24</v>
@@ -5027,13 +4978,13 @@
         <v>24</v>
       </c>
       <c r="N92" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O92" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P92" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O92" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P92" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q92" s="9"/>
       <c r="R92" s="10"/>
@@ -5062,13 +5013,13 @@
         <v>45058</v>
       </c>
       <c r="G93" s="8" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="H93" s="8" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="I93" s="8" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="J93" s="9" t="s">
         <v>24</v>
@@ -5081,13 +5032,13 @@
         <v>24</v>
       </c>
       <c r="N93" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O93" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P93" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O93" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P93" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q93" s="9"/>
       <c r="R93" s="10"/>
@@ -5116,13 +5067,13 @@
         <v>45058</v>
       </c>
       <c r="G94" s="8" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="H94" s="8" t="s">
         <v>125</v>
       </c>
       <c r="I94" s="8" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="J94" s="9" t="s">
         <v>24</v>
@@ -5135,13 +5086,13 @@
         <v>24</v>
       </c>
       <c r="N94" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O94" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P94" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O94" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P94" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q94" s="9"/>
       <c r="R94" s="10"/>
@@ -5170,13 +5121,13 @@
         <v>45058</v>
       </c>
       <c r="G95" s="8" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="H95" s="8" t="s">
-        <v>254</v>
+        <v>246</v>
       </c>
       <c r="I95" s="8" t="s">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="J95" s="9" t="s">
         <v>24</v>
@@ -5189,13 +5140,13 @@
         <v>24</v>
       </c>
       <c r="N95" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O95" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P95" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O95" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P95" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q95" s="9"/>
       <c r="R95" s="10"/>
@@ -5224,13 +5175,13 @@
         <v>45058</v>
       </c>
       <c r="G96" s="8" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="H96" s="8" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="I96" s="8" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="J96" s="9" t="s">
         <v>24</v>
@@ -5243,13 +5194,13 @@
         <v>24</v>
       </c>
       <c r="N96" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O96" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P96" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O96" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P96" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q96" s="9"/>
       <c r="R96" s="10"/>
@@ -5278,13 +5229,13 @@
         <v>45058</v>
       </c>
       <c r="G97" s="8" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="H97" s="8" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="I97" s="8" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="J97" s="9" t="s">
         <v>24</v>
@@ -5297,13 +5248,13 @@
         <v>24</v>
       </c>
       <c r="N97" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O97" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P97" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O97" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P97" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q97" s="9"/>
       <c r="R97" s="10"/>
@@ -5323,41 +5274,41 @@
         <v>37</v>
       </c>
       <c r="D98" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E98" s="6" t="s">
         <v>209</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>210</v>
       </c>
       <c r="F98" s="7">
         <v>45058</v>
       </c>
       <c r="G98" s="8" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H98" s="8" t="s">
-        <v>263</v>
+        <v>255</v>
       </c>
       <c r="I98" s="8" t="s">
-        <v>264</v>
+        <v>256</v>
       </c>
       <c r="J98" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K98" s="9"/>
       <c r="L98" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="M98" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="N98" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O98" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="P98" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O98" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="P98" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q98" s="9"/>
       <c r="R98" s="10"/>
@@ -5377,41 +5328,41 @@
         <v>37</v>
       </c>
       <c r="D99" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="E99" s="6" t="s">
         <v>211</v>
-      </c>
-      <c r="E99" s="6" t="s">
-        <v>212</v>
       </c>
       <c r="F99" s="7">
         <v>45058</v>
       </c>
       <c r="G99" s="8" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H99" s="8" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="I99" s="8" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="J99" s="9" t="s">
         <v>24</v>
       </c>
       <c r="K99" s="9"/>
       <c r="L99" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="M99" s="9" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="N99" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O99" s="9" t="s">
+        <v>278</v>
+      </c>
+      <c r="P99" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O99" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="P99" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q99" s="9"/>
       <c r="R99" s="10"/>
@@ -5440,13 +5391,13 @@
         <v>45058</v>
       </c>
       <c r="G100" s="8" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="H100" s="8" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="I100" s="8" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="J100" s="9" t="s">
         <v>24</v>
@@ -5459,13 +5410,13 @@
         <v>24</v>
       </c>
       <c r="N100" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O100" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P100" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O100" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P100" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q100" s="9"/>
       <c r="R100" s="10"/>
@@ -5494,13 +5445,13 @@
         <v>45058</v>
       </c>
       <c r="G101" s="8" t="s">
-        <v>271</v>
+        <v>263</v>
       </c>
       <c r="H101" s="8" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="I101" s="8" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="J101" s="9" t="s">
         <v>24</v>
@@ -5513,13 +5464,13 @@
         <v>24</v>
       </c>
       <c r="N101" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O101" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P101" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O101" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P101" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q101" s="9"/>
       <c r="R101" s="10"/>
@@ -5548,13 +5499,13 @@
         <v>45058</v>
       </c>
       <c r="G102" s="8" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="H102" s="8" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="I102" s="8" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="J102" s="9" t="s">
         <v>24</v>
@@ -5567,13 +5518,13 @@
         <v>24</v>
       </c>
       <c r="N102" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O102" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P102" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O102" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P102" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q102" s="9"/>
       <c r="R102" s="10"/>
@@ -5593,22 +5544,22 @@
         <v>37</v>
       </c>
       <c r="D103" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="E103" s="6" t="s">
         <v>213</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>214</v>
       </c>
       <c r="F103" s="7">
         <v>45058</v>
       </c>
       <c r="G103" s="8" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="H103" s="8" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="I103" s="8" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="J103" s="9" t="s">
         <v>24</v>
@@ -5621,13 +5572,13 @@
         <v>24</v>
       </c>
       <c r="N103" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O103" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P103" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O103" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P103" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q103" s="9"/>
       <c r="R103" s="10"/>
@@ -5656,13 +5607,13 @@
         <v>45058</v>
       </c>
       <c r="G104" s="8" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="H104" s="8" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="I104" s="8" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="J104" s="9" t="s">
         <v>24</v>
@@ -5675,13 +5626,13 @@
         <v>24</v>
       </c>
       <c r="N104" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O104" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P104" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O104" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P104" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q104" s="9"/>
       <c r="R104" s="10"/>
@@ -5701,20 +5652,20 @@
         <v>37</v>
       </c>
       <c r="D105" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="E105" s="6" t="s">
         <v>215</v>
-      </c>
-      <c r="E105" s="6" t="s">
-        <v>216</v>
       </c>
       <c r="F105" s="7"/>
       <c r="G105" s="8"/>
       <c r="H105" s="8"/>
       <c r="I105" s="8"/>
       <c r="J105" s="9" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="L105" s="9"/>
       <c r="M105" s="9"/>
@@ -5739,20 +5690,20 @@
         <v>37</v>
       </c>
       <c r="D106" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="E106" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="E106" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="F106" s="7"/>
       <c r="G106" s="8"/>
       <c r="H106" s="8"/>
       <c r="I106" s="8"/>
       <c r="J106" s="9" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="L106" s="9"/>
       <c r="M106" s="9"/>
@@ -5777,20 +5728,20 @@
         <v>37</v>
       </c>
       <c r="D107" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="E107" s="6" t="s">
         <v>219</v>
-      </c>
-      <c r="E107" s="6" t="s">
-        <v>220</v>
       </c>
       <c r="F107" s="7"/>
       <c r="G107" s="8"/>
       <c r="H107" s="8"/>
       <c r="I107" s="8"/>
       <c r="J107" s="9" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="K107" s="9" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="L107" s="9"/>
       <c r="M107" s="9"/>
@@ -5815,20 +5766,20 @@
         <v>37</v>
       </c>
       <c r="D108" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="E108" s="6" t="s">
         <v>221</v>
-      </c>
-      <c r="E108" s="6" t="s">
-        <v>222</v>
       </c>
       <c r="F108" s="7"/>
       <c r="G108" s="8"/>
       <c r="H108" s="8"/>
       <c r="I108" s="8"/>
       <c r="J108" s="9" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="K108" s="9" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="L108" s="9"/>
       <c r="M108" s="9"/>
@@ -5853,20 +5804,20 @@
         <v>37</v>
       </c>
       <c r="D109" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="E109" s="6" t="s">
         <v>223</v>
-      </c>
-      <c r="E109" s="6" t="s">
-        <v>224</v>
       </c>
       <c r="F109" s="7"/>
       <c r="G109" s="8"/>
       <c r="H109" s="8"/>
       <c r="I109" s="8"/>
       <c r="J109" s="9" t="s">
-        <v>293</v>
+        <v>280</v>
       </c>
       <c r="K109" s="9" t="s">
-        <v>294</v>
+        <v>281</v>
       </c>
       <c r="L109" s="9"/>
       <c r="M109" s="9"/>
@@ -5900,13 +5851,13 @@
         <v>45058</v>
       </c>
       <c r="G110" s="8" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="H110" s="8" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="I110" s="8" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="J110" s="9" t="s">
         <v>24</v>
@@ -5919,13 +5870,13 @@
         <v>24</v>
       </c>
       <c r="N110" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="O110" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="P110" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="O110" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="P110" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="Q110" s="9"/>
       <c r="R110" s="10"/>

</xml_diff>